<commit_message>
FadeIn, Out 오류 수정
맵 변경시 여러번 실행되는 오류 수정
</commit_message>
<xml_diff>
--- a/Excel2Json/bin/ep00/ep00.xlsx
+++ b/Excel2Json/bin/ep00/ep00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Slanted_Structure\Excel2Json\bin\ep00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC05700-346C-489E-BD11-5BBD8AA84556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3A4E35-5A3E-4B5C-85EB-BA7539FFEF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="6" activeTab="13" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="6" activeTab="14" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="001010_task" sheetId="15" r:id="rId1"/>
@@ -323,7 +323,8 @@
 FadeIn = 9
 FadeOut=10
 Cinematic = 11
-EndingChoice=12</t>
+EndingChoice=12
+Clear = 13</t>
         </r>
       </text>
     </comment>
@@ -2340,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACEF5D3A-0E1E-4C46-9D07-F45230D15113}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2488,7 +2489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30E00E-1A2F-4A71-B81B-26375E330124}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -2786,16 +2789,17 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="24.19921875" customWidth="1"/>
-    <col min="4" max="4" width="60.59765625" customWidth="1"/>
-    <col min="5" max="5" width="47.69921875" customWidth="1"/>
+    <col min="1" max="1" width="17.59765625" customWidth="1"/>
+    <col min="2" max="2" width="28.09765625" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="4" max="4" width="19.09765625" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
@@ -3569,7 +3573,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Dove 이미지 수정, 002020_pimp 대사 추가
</commit_message>
<xml_diff>
--- a/Excel2Json/bin/ep00/ep00.xlsx
+++ b/Excel2Json/bin/ep00/ep00.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justb\GitHub\Slanted_Structure\Excel2Json\bin\ep00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABECADA-0D09-4345-ABF0-1C58BAFEA156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9B18FD-9082-4C78-AF13-8B34DFCC5DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="3" activeTab="4" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="6" activeTab="11" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
   <sheets>
     <sheet name="001010_task" sheetId="15" r:id="rId1"/>
@@ -24,11 +24,12 @@
     <sheet name="002011_task" sheetId="17" r:id="rId9"/>
     <sheet name="002011" sheetId="8" r:id="rId10"/>
     <sheet name="002020_1" sheetId="9" r:id="rId11"/>
-    <sheet name="002020_2" sheetId="12" r:id="rId12"/>
-    <sheet name="002030_1" sheetId="10" r:id="rId13"/>
-    <sheet name="002030_2" sheetId="11" r:id="rId14"/>
-    <sheet name="002030_3_task" sheetId="22" r:id="rId15"/>
-    <sheet name="002030_3" sheetId="14" r:id="rId16"/>
+    <sheet name="002020_pimp" sheetId="24" r:id="rId12"/>
+    <sheet name="002020_2" sheetId="12" r:id="rId13"/>
+    <sheet name="002030_1" sheetId="10" r:id="rId14"/>
+    <sheet name="002030_2" sheetId="11" r:id="rId15"/>
+    <sheet name="002030_3_task" sheetId="22" r:id="rId16"/>
+    <sheet name="002030_3" sheetId="14" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -523,6 +524,265 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>최선</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{F9D93E4E-30AF-4ACF-927A-328E65CE5A8B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">0: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">기본
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>화난</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">표정
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>예민한</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">표정
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>슬픈</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">표정
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>놀란</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">액션
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">패닉
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">6: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>우는</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">표정
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>최선</author>
     <author>훠이</author>
   </authors>
   <commentList>
@@ -732,7 +992,7 @@
 </comments>
 </file>
 
-<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>최선</author>
@@ -2524,7 +2784,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="109">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2899,6 +3159,42 @@
   </si>
   <si>
     <t>약해 보이는데... 한 번 차볼까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잡았다…! 어딜 도망가…!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이거 놔…!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포주</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빚도 안 갚고 어딜 도망가려고 해? 기껏 돈벌게 해줬더니 건방진 X…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너는 오늘 죽는 줄 알아.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>???는 포주들에게 끌려가다가 문득 자신이 가지고 있는 초능력이 있다는 것을 깨달았고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신의 초능력을 이용해서 포주들에게서 벗어나 다시 도망치기 시작했다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어어? 뭐야? 어떻게 된거야? 거기 안서???</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002020_pimp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3454,7 +3750,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3730,6 +4026,178 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6716454B-9484-4D14-BA08-B5A4B46F4B74}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E17" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E0410B-99B7-4713-80E6-B6B994BDC0E7}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -3853,7 +4321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BCAD07-2A0E-4763-A06C-AEF4838FA08B}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -3983,7 +4451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D03DFD-04FF-49B1-A1C2-B442B1027B55}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -4102,7 +4570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACEF5D3A-0E1E-4C46-9D07-F45230D15113}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -4234,7 +4702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30E00E-1A2F-4A71-B81B-26375E330124}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -4814,7 +5282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F51F5BB-4798-4887-95FF-B169D0EB787A}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>